<commit_message>
merge report and change position of minutes template
</commit_message>
<xml_diff>
--- a/document/Task.xlsx
+++ b/document/Task.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="120">
   <si>
     <t>No.</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Delete field type</t>
   </si>
   <si>
-    <t>View field timeline</t>
-  </si>
-  <si>
     <t xml:space="preserve">Payment </t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>Percentage revenue from field's price</t>
   </si>
   <si>
-    <t>Revenue statistical</t>
-  </si>
-  <si>
     <t>Edit profile</t>
   </si>
   <si>
@@ -323,12 +317,6 @@
     <t>4/Giá sân và giá cho từng khung giờ chủ sân set khác nhau</t>
   </si>
   <si>
-    <t>5/ Khi nào thì người chơi thực hiện trả phí</t>
-  </si>
-  <si>
-    <t>6/ Khi nào thì chuyển tiền cho chủ sân</t>
-  </si>
-  <si>
     <t>2/ Paypal để thanh toán</t>
   </si>
   <si>
@@ -336,9 +324,6 @@
   </si>
   <si>
     <t>7/ Thời gian chờ cáp kèo là bao lâu, sẽ hủy nếu ko tìm ra người chơi, phục vụ cho người chơi khác trước khi trận đấu bắt đầu bao lâu?</t>
-  </si>
-  <si>
-    <t>8/ Nếu cáp kèo và chuyển phí rồi mà cancel thì sẽ hồi bao nhiêu phí và phải thực hiện trước khi trận đấu diễn ra là bao lâu?</t>
   </si>
   <si>
     <t>3/ Timeline của chủ sân là timeline cho từng sân, timeline cho người dùng là timeline cho một cụm sân</t>
@@ -367,6 +352,39 @@
   </si>
   <si>
     <t>HuanPM</t>
+  </si>
+  <si>
+    <t>8/ Nếu cáp kèo và chuyển phí rồi mà cancel thì sẽ hồi bao nhiêu phí và phải thực hiện trước khi trận đấu diễn ra là bao lâu, người chơi bị cancel kèo sẽ được matching với trận đấu khác như thế nào?</t>
+  </si>
+  <si>
+    <t>6/ Khi nào thì chuyển tiền cho chủ sân?</t>
+  </si>
+  <si>
+    <t>5/ Khi nào thì người chơi thực hiện trả phí đối với kèo cáp, có nên trả trước ko hay đợi 2 bên cùng đồng ý rồi trả, nên trả 1 nửa rồi chia lại đối với kèo có cược hay sao?</t>
+  </si>
+  <si>
+    <t>Admin receive request about field owner and verfify to create field for field owner</t>
+  </si>
+  <si>
+    <t>Change type of field</t>
+  </si>
+  <si>
+    <t>When field owner request, remove field from field list of field owener</t>
+  </si>
+  <si>
+    <t>Field type: 5vs5, 7vs7, 11vs11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commissions from field price </t>
+  </si>
+  <si>
+    <t>Sales statistical</t>
+  </si>
+  <si>
+    <t>For date, for month, for year</t>
+  </si>
+  <si>
+    <t>10/ Tìm kiếm người chơi unfair thì có cần confirm từ bên request đặt sân trước hay ko?</t>
   </si>
 </sst>
 </file>
@@ -977,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,7 +1015,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D1" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1017,10 +1035,10 @@
         <v>17</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>21</v>
@@ -1031,7 +1049,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>4</v>
@@ -1040,14 +1058,14 @@
         <v>7</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F4" s="8">
         <v>1</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1071,7 +1089,7 @@
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
       <c r="D6" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="8"/>
@@ -1104,14 +1122,14 @@
         <v>37</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F8" s="8">
         <v>3</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="10" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1140,14 +1158,14 @@
         <v>28</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" s="20">
         <v>1</v>
       </c>
       <c r="G10" s="9"/>
       <c r="H10" s="21" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -1157,19 +1175,19 @@
       <c r="B11" s="11"/>
       <c r="C11" s="19"/>
       <c r="D11" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F11" s="20">
         <v>1</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1179,17 +1197,17 @@
       <c r="B12" s="11"/>
       <c r="C12" s="19"/>
       <c r="D12" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F12" s="8">
         <v>1</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1199,10 +1217,10 @@
       <c r="B13" s="11"/>
       <c r="C13" s="19"/>
       <c r="D13" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="14"/>
@@ -1214,20 +1232,20 @@
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F14" s="8">
         <v>1</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="10" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1237,10 +1255,10 @@
       <c r="B15" s="11"/>
       <c r="C15" s="23"/>
       <c r="D15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>63</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="14"/>
@@ -1253,7 +1271,7 @@
       <c r="B16" s="11"/>
       <c r="C16" s="24"/>
       <c r="D16" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="8"/>
@@ -1272,14 +1290,14 @@
         <v>32</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F17" s="8">
         <v>2</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1289,10 +1307,10 @@
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
       <c r="D18" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="14"/>
@@ -1308,7 +1326,7 @@
         <v>33</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="14"/>
@@ -1326,14 +1344,14 @@
         <v>30</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F20" s="8">
         <v>2</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="25" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1343,10 +1361,10 @@
       <c r="B21" s="11"/>
       <c r="C21" s="15"/>
       <c r="D21" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="14"/>
@@ -1393,13 +1411,13 @@
         <v>21</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>20</v>
@@ -1409,7 +1427,7 @@
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="25" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1460,20 +1478,20 @@
       </c>
       <c r="B28" s="36"/>
       <c r="C28" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>39</v>
       </c>
       <c r="E28" s="38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F28" s="39">
         <v>1</v>
       </c>
       <c r="G28" s="40"/>
       <c r="H28" s="10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1483,10 +1501,10 @@
       <c r="B29" s="36"/>
       <c r="C29" s="11"/>
       <c r="D29" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="42" t="s">
         <v>77</v>
-      </c>
-      <c r="E29" s="42" t="s">
-        <v>79</v>
       </c>
       <c r="F29" s="39"/>
       <c r="G29" s="14"/>
@@ -1499,17 +1517,17 @@
       <c r="B30" s="36"/>
       <c r="C30" s="11"/>
       <c r="D30" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F30" s="8">
         <v>1</v>
       </c>
       <c r="G30" s="14"/>
       <c r="H30" s="10" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1519,10 +1537,10 @@
       <c r="B31" s="36"/>
       <c r="C31" s="11"/>
       <c r="D31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="44" t="s">
         <v>78</v>
-      </c>
-      <c r="E31" s="44" t="s">
-        <v>80</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="14"/>
@@ -1535,10 +1553,10 @@
       <c r="B32" s="36"/>
       <c r="C32" s="11"/>
       <c r="D32" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E32" s="44" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="14"/>
@@ -1551,10 +1569,10 @@
       <c r="B33" s="36"/>
       <c r="C33" s="11"/>
       <c r="D33" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E33" s="45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="14"/>
@@ -1562,337 +1580,340 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B34" s="36"/>
-      <c r="C34" s="11"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="44"/>
-      <c r="F34" s="8"/>
+        <v>34</v>
+      </c>
+      <c r="E34" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" s="46">
+        <v>2</v>
+      </c>
       <c r="G34" s="14"/>
-      <c r="H34" s="10"/>
+      <c r="H34" s="47" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B35" s="36"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="5" t="s">
+      <c r="C35" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="48">
+        <v>4</v>
+      </c>
+      <c r="G35" s="29"/>
+      <c r="H35" s="49"/>
+    </row>
+    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
         <v>34</v>
       </c>
-      <c r="E35" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="F35" s="46">
-        <v>2</v>
-      </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="47" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
-        <v>33</v>
-      </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F36" s="48">
-        <v>4</v>
-      </c>
-      <c r="G36" s="29"/>
-      <c r="H36" s="49"/>
-    </row>
-    <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B36" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="50">
+        <v>1</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
-        <v>34</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>14</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="5" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" s="50">
-        <v>1</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F37" s="51"/>
       <c r="G37" s="13"/>
-      <c r="H37" s="10" t="s">
-        <v>112</v>
-      </c>
+      <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
+      <c r="C38" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="D38" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="51"/>
+        <v>43</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="50">
+        <v>2</v>
+      </c>
       <c r="G38" s="13"/>
-      <c r="H38" s="10"/>
+      <c r="H38" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B39" s="19"/>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="15"/>
+      <c r="D39" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="E39" s="13"/>
-      <c r="F39" s="50">
-        <v>2</v>
-      </c>
+      <c r="F39" s="51"/>
       <c r="G39" s="13"/>
-      <c r="H39" s="25" t="s">
-        <v>112</v>
-      </c>
+      <c r="H39" s="26"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B40" s="19"/>
-      <c r="C40" s="15"/>
+      <c r="C40" s="7" t="s">
+        <v>16</v>
+      </c>
       <c r="D40" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E40" s="13"/>
-      <c r="F40" s="51"/>
+      <c r="F40" s="50">
+        <v>2</v>
+      </c>
       <c r="G40" s="13"/>
-      <c r="H40" s="26"/>
+      <c r="H40" s="25" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" s="19"/>
-      <c r="C41" s="7" t="s">
-        <v>16</v>
-      </c>
+      <c r="C41" s="15"/>
       <c r="D41" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E41" s="13"/>
-      <c r="F41" s="50">
-        <v>2</v>
-      </c>
+      <c r="F41" s="51"/>
       <c r="G41" s="13"/>
-      <c r="H41" s="25" t="s">
+      <c r="H41" s="26"/>
+    </row>
+    <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="5">
+        <v>40</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" s="5">
-        <v>39</v>
-      </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="26"/>
+      <c r="F42" s="8">
+        <v>1</v>
+      </c>
+      <c r="G42" s="14"/>
+      <c r="H42" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
-        <v>40</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="D43" s="41" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" s="18"/>
-      <c r="F43" s="8">
-        <v>1</v>
-      </c>
+      <c r="E43" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F43" s="8"/>
       <c r="G43" s="14"/>
-      <c r="H43" s="10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H43" s="10"/>
+    </row>
+    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
       <c r="D44" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="18"/>
+        <v>40</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>114</v>
+      </c>
       <c r="F44" s="8"/>
       <c r="G44" s="14"/>
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
-      <c r="D45" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="E45" s="18"/>
+      <c r="D45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" s="18" t="s">
+        <v>115</v>
+      </c>
       <c r="F45" s="8"/>
       <c r="G45" s="14"/>
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
       <c r="D46" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E46" s="18"/>
+        <v>94</v>
+      </c>
+      <c r="E46" s="13"/>
       <c r="F46" s="8"/>
       <c r="G46" s="14"/>
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="8"/>
+      <c r="C47" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F47" s="8">
+        <v>3</v>
+      </c>
       <c r="G47" s="14"/>
-      <c r="H47" s="10"/>
+      <c r="H47" s="25" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="5">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B48" s="19"/>
-      <c r="C48" s="19" t="s">
-        <v>48</v>
-      </c>
+      <c r="C48" s="19"/>
       <c r="D48" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="E48" s="13"/>
-      <c r="F48" s="8">
-        <v>3</v>
-      </c>
-      <c r="G48" s="14"/>
-      <c r="H48" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E48" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="F48" s="8"/>
+      <c r="G48" s="41"/>
+      <c r="H48" s="26"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" s="52" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D52" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D53" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D54" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D55" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D56" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="5">
-        <v>46</v>
-      </c>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="41" t="s">
-        <v>50</v>
-      </c>
-      <c r="E49" s="41"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="41"/>
-      <c r="H49" s="26"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D51" s="52" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D52" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D53" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D54" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D55" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D56" s="1" t="s">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D57" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D57" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D58" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D59" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D60" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D62" s="1" t="s">
-        <v>106</v>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="51">
     <mergeCell ref="H28:H29"/>
-    <mergeCell ref="H30:H34"/>
+    <mergeCell ref="H30:H33"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="C20:C21"/>
@@ -1900,48 +1921,48 @@
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="H24:H27"/>
     <mergeCell ref="H22:H23"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="F22:F23"/>
     <mergeCell ref="H4:H7"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="H17:H19"/>
-    <mergeCell ref="H20:H21"/>
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C28:C35"/>
-    <mergeCell ref="B43:B49"/>
-    <mergeCell ref="C48:C49"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="B42:B48"/>
+    <mergeCell ref="C47:C48"/>
     <mergeCell ref="E24:E27"/>
-    <mergeCell ref="C43:C47"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="C36:C37"/>
     <mergeCell ref="B4:B23"/>
-    <mergeCell ref="B24:B36"/>
+    <mergeCell ref="B24:B35"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="C40:C41"/>
     <mergeCell ref="F4:F7"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="F17:F19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F30:F34"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F43:F47"/>
-    <mergeCell ref="F48:F49"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="H43:H47"/>
-    <mergeCell ref="H48:H49"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F42:F46"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="H42:H46"/>
+    <mergeCell ref="H47:H48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
commit after Mr.Khanh review
</commit_message>
<xml_diff>
--- a/document/Task.xlsx
+++ b/document/Task.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="124">
   <si>
     <t>No.</t>
   </si>
@@ -385,6 +385,18 @@
   </si>
   <si>
     <t>10/ Tìm kiếm người chơi unfair thì có cần confirm từ bên request đặt sân trước hay ko?</t>
+  </si>
+  <si>
+    <t>Thông báo promotion đến người dùng</t>
+  </si>
+  <si>
+    <t>Người dùng nhập thời gian muốn đá -&gt; lựa chọn -&gt; ko có thì mới view timeline</t>
+  </si>
+  <si>
+    <t>Giá sân và promotion do chủ quyết định</t>
+  </si>
+  <si>
+    <t>Matching đến sân bất kỳ phù hợp</t>
   </si>
 </sst>
 </file>
@@ -995,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1910,28 +1922,43 @@
         <v>101</v>
       </c>
     </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D69" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D70" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="H30:H33"/>
-    <mergeCell ref="C10:C13"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F30:F33"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="H4:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="H42:H46"/>
+    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F42:F46"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="F17:F19"/>
     <mergeCell ref="E4:E7"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="C14:C16"/>
@@ -1948,21 +1975,26 @@
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C38:C39"/>
     <mergeCell ref="C40:C41"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F42:F46"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="H42:H46"/>
-    <mergeCell ref="H47:H48"/>
+    <mergeCell ref="H4:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F30:F33"/>
+    <mergeCell ref="F22:F23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>